<commit_message>
add day 23 to do list
</commit_message>
<xml_diff>
--- a/PaperImplementationPlan.xlsx
+++ b/PaperImplementationPlan.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/WIND/GlodonWorkSpace/GlodonTemp/LHMTempPaper/TEMPpaper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaishai\Desktop\11.5\123\TEMPpaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="720" windowWidth="24020" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="2055" yWindow="720" windowWidth="24015" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2018-31-stage" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>日期</t>
   </si>
@@ -148,7 +145,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="DengXian"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -223,13 +220,21 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
+        <rFont val="DengXian"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 2.一个版本 v1.0的摘要</t>
     </r>
+  </si>
+  <si>
+    <t>1.阅读1月22日下载的文献，简要说明主要内容                                            2.未完成目录摘要</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.继续对这发现相似性的这几篇文章进行阅读，从这些论文的参考文献中检索一些国内外的其他文章，寻找其他的相关内容；</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -237,20 +242,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -258,7 +263,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -266,7 +271,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -277,21 +282,21 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="DengXian"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,7 +314,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,6 +322,13 @@
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,13 +369,13 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -372,9 +384,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -387,26 +403,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -686,23 +698,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="59.5" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="7" max="7" width="56.5" customWidth="1"/>
-    <col min="8" max="8" width="56.5" style="13" customWidth="1"/>
-    <col min="9" max="9" width="30.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="56.5" style="8" customWidth="1"/>
+    <col min="9" max="9" width="30.875" customWidth="1"/>
+    <col min="10" max="10" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -724,7 +736,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -803,17 +815,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:33" s="2" customFormat="1" ht="154.5" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="10">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="1">
@@ -825,18 +837,18 @@
       <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+    <row r="3" spans="1:33" s="2" customFormat="1" ht="108" customHeight="1">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="1">
         <v>43123</v>
       </c>
@@ -846,32 +858,34 @@
       <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="I3" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" s="2" customFormat="1" ht="47.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="1">
         <v>43124</v>
       </c>
       <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="2">
-        <v>3</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:33" s="2" customFormat="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="1">
         <v>43125</v>
       </c>
@@ -881,13 +895,13 @@
       <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:33" s="2" customFormat="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="1">
         <v>43126</v>
       </c>
@@ -897,13 +911,13 @@
       <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:33" s="2" customFormat="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="1">
         <v>43127</v>
       </c>
@@ -913,13 +927,13 @@
       <c r="G7" s="2">
         <v>6</v>
       </c>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:33" s="2" customFormat="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="1">
         <v>43128</v>
       </c>
@@ -929,13 +943,13 @@
       <c r="G8" s="2">
         <v>7</v>
       </c>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:33" s="2" customFormat="1">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1">
@@ -947,13 +961,13 @@
       <c r="G9" s="2">
         <v>8</v>
       </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:33" s="2" customFormat="1">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1">
         <v>43130</v>
       </c>
@@ -963,13 +977,13 @@
       <c r="G10" s="2">
         <v>9</v>
       </c>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:33" s="2" customFormat="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1">
         <v>43131</v>
       </c>
@@ -979,13 +993,13 @@
       <c r="G11" s="2">
         <v>10</v>
       </c>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:33" s="2" customFormat="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1">
         <v>43132</v>
       </c>
@@ -995,13 +1009,13 @@
       <c r="G12" s="2">
         <v>11</v>
       </c>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:33" s="2" customFormat="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="1">
         <v>43133</v>
       </c>
@@ -1011,13 +1025,13 @@
       <c r="G13" s="2">
         <v>12</v>
       </c>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:33" s="2" customFormat="1">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="1">
         <v>43134</v>
       </c>
@@ -1027,13 +1041,13 @@
       <c r="G14" s="2">
         <v>13</v>
       </c>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:33" s="2" customFormat="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="1">
         <v>43135</v>
       </c>
@@ -1043,15 +1057,15 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:33" s="2" customFormat="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10">
         <v>3</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="10">
         <v>6</v>
       </c>
       <c r="E16" s="1">
@@ -1063,13 +1077,13 @@
       <c r="G16" s="2">
         <v>15</v>
       </c>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="1">
         <v>43137</v>
       </c>
@@ -1079,13 +1093,13 @@
       <c r="G17" s="2">
         <v>16</v>
       </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="1">
         <v>43138</v>
       </c>
@@ -1095,13 +1109,13 @@
       <c r="G18" s="2">
         <v>17</v>
       </c>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="1">
         <v>43139</v>
       </c>
@@ -1111,13 +1125,13 @@
       <c r="G19" s="2">
         <v>18</v>
       </c>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="1">
         <v>43140</v>
       </c>
@@ -1127,13 +1141,13 @@
       <c r="G20" s="2">
         <v>19</v>
       </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="1">
         <v>43141</v>
       </c>
@@ -1143,13 +1157,13 @@
       <c r="G21" s="2">
         <v>20</v>
       </c>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="1">
         <v>43142</v>
       </c>
@@ -1159,13 +1173,13 @@
       <c r="G22" s="2">
         <v>21</v>
       </c>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10">
         <v>7</v>
       </c>
       <c r="E23" s="3">
@@ -1177,13 +1191,13 @@
       <c r="G23" s="2">
         <v>22</v>
       </c>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="3">
         <v>43144</v>
       </c>
@@ -1193,13 +1207,13 @@
       <c r="G24" s="2">
         <v>23</v>
       </c>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="3">
         <v>43145</v>
       </c>
@@ -1209,13 +1223,13 @@
       <c r="G25" s="2">
         <v>24</v>
       </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="3">
         <v>43146</v>
       </c>
@@ -1225,13 +1239,13 @@
       <c r="G26" s="2">
         <v>25</v>
       </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="3">
         <v>43147</v>
       </c>
@@ -1241,13 +1255,13 @@
       <c r="G27" s="2">
         <v>26</v>
       </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="3">
         <v>43148</v>
       </c>
@@ -1257,13 +1271,13 @@
       <c r="G28" s="2">
         <v>27</v>
       </c>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="3">
         <v>43149</v>
       </c>
@@ -1273,17 +1287,17 @@
       <c r="G29" s="2">
         <v>28</v>
       </c>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7" t="s">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="3">
@@ -1295,13 +1309,13 @@
       <c r="G30" s="2">
         <v>29</v>
       </c>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="3">
         <v>43151</v>
       </c>
@@ -1311,13 +1325,13 @@
       <c r="G31" s="2">
         <v>30</v>
       </c>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="3">
         <v>43152</v>
       </c>
@@ -1327,13 +1341,13 @@
       <c r="G32" s="2">
         <v>31</v>
       </c>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="3">
         <v>43153</v>
       </c>
@@ -1343,13 +1357,13 @@
       <c r="G33" s="2">
         <v>32</v>
       </c>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
       <c r="E34" s="1">
         <v>43154</v>
       </c>
@@ -1359,13 +1373,13 @@
       <c r="G34" s="2">
         <v>33</v>
       </c>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="1">
         <v>43155</v>
       </c>
@@ -1375,13 +1389,13 @@
       <c r="G35" s="2">
         <v>34</v>
       </c>
-      <c r="H35" s="11"/>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="1">
         <v>43156</v>
       </c>
@@ -1391,7 +1405,7 @@
       <c r="G36" s="2">
         <v>35</v>
       </c>
-      <c r="H36" s="11"/>
+      <c r="H36" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
add day 28 plan
</commit_message>
<xml_diff>
--- a/PaperImplementationPlan.xlsx
+++ b/PaperImplementationPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>日期</t>
   </si>
@@ -255,6 +255,14 @@
   </si>
   <si>
     <t>继续查找资料，明晰论文研究背景</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不断查找资料的过程中，对研究的问题有了进一步认识</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>将开始4篇论文中的剩余两篇的参考文献下载下来</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -723,7 +731,7 @@
   <dimension ref="A1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -922,6 +930,9 @@
         <v>23</v>
       </c>
       <c r="H5" s="6"/>
+      <c r="I5" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:33" s="2" customFormat="1" ht="31.5">
       <c r="A6" s="12"/>
@@ -938,6 +949,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="6"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:33" s="2" customFormat="1">
       <c r="A7" s="12"/>
@@ -954,8 +966,9 @@
         <v>25</v>
       </c>
       <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:33" s="2" customFormat="1">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:33" s="2" customFormat="1" ht="31.5">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -966,8 +979,8 @@
       <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" s="2">
-        <v>7</v>
+      <c r="G8" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="H8" s="6"/>
     </row>
@@ -1434,7 +1447,8 @@
       <c r="H36" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="I5:I7"/>
     <mergeCell ref="D30:D36"/>
     <mergeCell ref="A2:A36"/>
     <mergeCell ref="B2:B29"/>

</xml_diff>